<commit_message>
Sheet tests and row count fix
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAB2EE4-9F19-4777-9371-C86757FE281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F191C-979E-4517-9D4D-F6D49C5B6978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="21792" windowHeight="12468" activeTab="1" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,9 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFD262-07B1-49C8-A4BA-BD18114D64AA}">
   <dimension ref="A10:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -485,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2B282D-E29C-4833-BC0D-3206BC8B9899}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add some more existing file tests and restructure to allow for append.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F191C-979E-4517-9D4D-F6D49C5B6978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919B676-E876-42C0-8C93-673CEA7D64F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Another" sheetId="2" r:id="rId2"/>
+    <sheet name="NoHeaders" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="myData">Sheet1!$A$10:$C$13</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Test</t>
   </si>
@@ -426,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFD262-07B1-49C8-A4BA-BD18114D64AA}">
   <dimension ref="A10:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -484,7 +485,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,4 +549,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2D721F-E695-46EA-89D5-1CEEB5C37595}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Append support to Excel.Write (#3558)
Adds support for appending to an existing Excel table.

# Important Notes
- Renamed `Column_Mapping` to `Column_Name_Mapping`
- Changed new type name to `Map_Column`
- Added last modified time and creation time to `File`.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F191C-979E-4517-9D4D-F6D49C5B6978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919B676-E876-42C0-8C93-673CEA7D64F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Another" sheetId="2" r:id="rId2"/>
+    <sheet name="NoHeaders" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="myData">Sheet1!$A$10:$C$13</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Test</t>
   </si>
@@ -426,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFD262-07B1-49C8-A4BA-BD18114D64AA}">
   <dimension ref="A10:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -484,7 +485,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,4 +549,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2D721F-E695-46EA-89D5-1CEEB5C37595}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Additional tests. Fix Image warning. Use NameDeduplication when reading in existing table.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25505"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919B676-E876-42C0-8C93-673CEA7D64F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2C6DDB-A985-4548-A388-FAF3C5C19014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Another" sheetId="2" r:id="rId2"/>
     <sheet name="NoHeaders" sheetId="3" r:id="rId3"/>
+    <sheet name="Random" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="myData">Sheet1!$A$10:$C$13</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>Test</t>
   </si>
@@ -73,6 +74,18 @@
   </si>
   <si>
     <t>DD</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -485,7 +498,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A2:D4"/>
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2D721F-E695-46EA-89D5-1CEEB5C37595}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
@@ -606,4 +619,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9178A76A-1B87-40F9-8AD1-4F2166D406F2}">
+  <dimension ref="B3:V12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:V6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44715</v>
+      </c>
+      <c r="S4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44693</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44607</v>
+      </c>
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel test sheets.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2C6DDB-A985-4548-A388-FAF3C5C19014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5CA6D1-A1C4-42DD-9AED-4BBAC77BF70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="16200" windowHeight="10128" activeTab="3" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>Test</t>
   </si>
@@ -626,7 +626,7 @@
   <dimension ref="B3:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:V6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,13 +736,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">

</xml_diff>

<commit_message>
Additional tests for Excel Append (#3580)
Add some additional scenarios to Excel append tests:
- Non-A1 start
- Name duplication
- Hitting another range

# Important Notes
Also fixed a warning in the Image library.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25505"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919B676-E876-42C0-8C93-673CEA7D64F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5CA6D1-A1C4-42DD-9AED-4BBAC77BF70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="16200" windowHeight="10128" activeTab="3" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Another" sheetId="2" r:id="rId2"/>
     <sheet name="NoHeaders" sheetId="3" r:id="rId3"/>
+    <sheet name="Random" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="myData">Sheet1!$A$10:$C$13</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>Test</t>
   </si>
@@ -73,6 +74,18 @@
   </si>
   <si>
     <t>DD</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -485,7 +498,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A2:D4"/>
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2D721F-E695-46EA-89D5-1CEEB5C37595}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
@@ -606,4 +619,187 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9178A76A-1B87-40F9-8AD1-4F2166D406F2}">
+  <dimension ref="B3:V12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44715</v>
+      </c>
+      <c r="S4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44693</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44607</v>
+      </c>
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Date, Time_Of_Day and Date_Time support to Excel.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5CA6D1-A1C4-42DD-9AED-4BBAC77BF70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4DC43B-541B-4124-8D92-0DDC01DF2D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="16200" windowHeight="10128" activeTab="3" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="22050" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,6 +92,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="d\-mmm\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,9 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,13 +444,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFD262-07B1-49C8-A4BA-BD18114D64AA}">
-  <dimension ref="A10:C13"/>
+  <dimension ref="A10:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -454,8 +465,15 @@
       <c r="C10" s="1">
         <v>44724</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>0.52425925925925931</v>
+      </c>
+      <c r="E10" s="4">
+        <f>C10+D10</f>
+        <v>44724.524259259262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -465,8 +483,15 @@
       <c r="C11" s="1">
         <v>44854</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>5.8159722222222217E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" ref="E11:E13" si="0">C11+D11</f>
+        <v>44854.058159722219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -476,8 +501,15 @@
       <c r="C12" s="1">
         <v>44772</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="3">
+        <v>0.11527777777777777</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>44772.115277777775</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -487,9 +519,17 @@
       <c r="C13" s="1">
         <v>44849</v>
       </c>
+      <c r="D13" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>44849.375</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -501,9 +541,9 @@
       <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -531,7 +571,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -545,7 +585,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -572,9 +612,9 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -588,7 +628,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -602,7 +642,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -625,13 +665,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9178A76A-1B87-40F9-8AD1-4F2166D406F2}">
   <dimension ref="B3:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -657,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -683,7 +723,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -709,7 +749,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -735,7 +775,7 @@
         <v>44607</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -743,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K9" t="s">
         <v>4</v>
       </c>
@@ -757,7 +797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K10" t="s">
         <v>12</v>
       </c>
@@ -771,7 +811,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K11" t="s">
         <v>13</v>
       </c>
@@ -785,7 +825,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K12" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Adds Date, Time_Of_Day and Date_Time support to Excel IO (#3997)
- Allow date time inputs from Excel.
- Enables disabled test.
- Fix for Map.==.
- Allow nulls in crosstab name.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/TestSheet.xlsx
+++ b/test/Table_Tests/data/TestSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5CA6D1-A1C4-42DD-9AED-4BBAC77BF70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4DC43B-541B-4124-8D92-0DDC01DF2D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="16200" windowHeight="10128" activeTab="3" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
+    <workbookView xWindow="22050" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E8335DB9-710D-430A-BBED-D81064B2E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,6 +92,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="d\-mmm\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,9 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,13 +444,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFD262-07B1-49C8-A4BA-BD18114D64AA}">
-  <dimension ref="A10:C13"/>
+  <dimension ref="A10:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -454,8 +465,15 @@
       <c r="C10" s="1">
         <v>44724</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>0.52425925925925931</v>
+      </c>
+      <c r="E10" s="4">
+        <f>C10+D10</f>
+        <v>44724.524259259262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -465,8 +483,15 @@
       <c r="C11" s="1">
         <v>44854</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>5.8159722222222217E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" ref="E11:E13" si="0">C11+D11</f>
+        <v>44854.058159722219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -476,8 +501,15 @@
       <c r="C12" s="1">
         <v>44772</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="3">
+        <v>0.11527777777777777</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>44772.115277777775</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -487,9 +519,17 @@
       <c r="C13" s="1">
         <v>44849</v>
       </c>
+      <c r="D13" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>44849.375</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -501,9 +541,9 @@
       <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -531,7 +571,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -545,7 +585,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -572,9 +612,9 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -588,7 +628,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -602,7 +642,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -625,13 +665,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9178A76A-1B87-40F9-8AD1-4F2166D406F2}">
   <dimension ref="B3:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -657,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -683,7 +723,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -709,7 +749,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -735,7 +775,7 @@
         <v>44607</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -743,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K9" t="s">
         <v>4</v>
       </c>
@@ -757,7 +797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K10" t="s">
         <v>12</v>
       </c>
@@ -771,7 +811,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K11" t="s">
         <v>13</v>
       </c>
@@ -785,7 +825,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="K12" t="s">
         <v>14</v>
       </c>

</xml_diff>